<commit_message>
Add new excel - planned UC
</commit_message>
<xml_diff>
--- a/usecases/Usecase doc.xlsx
+++ b/usecases/Usecase doc.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,7 +11,7 @@
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -697,6 +697,9 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -706,12 +709,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -728,7 +728,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
@@ -820,7 +820,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-684E-462E-B6C5-08C4C156CB9E}"/>
             </c:ext>
@@ -928,7 +928,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
@@ -1015,6 +1015,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3913-4CCA-937B-BFE2918FD451}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1084,6 +1089,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3913-4CCA-937B-BFE2918FD451}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -1153,6 +1163,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-3913-4CCA-937B-BFE2918FD451}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1280,9 +1295,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1320,9 +1335,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1357,7 +1372,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1392,7 +1407,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1572,7 +1587,7 @@
   <dimension ref="C1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="W4" sqref="W4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1730,15 +1745,15 @@
       </c>
     </row>
     <row r="8" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="45" t="s">
+      <c r="C8" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="48"/>
     </row>
     <row r="9" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C9" s="18">
@@ -1933,12 +1948,12 @@
       </c>
     </row>
     <row r="28" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C28" s="48" t="s">
+      <c r="C28" s="45" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="29" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C29" s="48" t="s">
+      <c r="C29" s="45" t="s">
         <v>29</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add total time in UC DOC
</commit_message>
<xml_diff>
--- a/usecases/Usecase doc.xlsx
+++ b/usecases/Usecase doc.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,7 +11,7 @@
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -108,8 +108,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,6 +140,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -149,7 +156,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="36">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -577,6 +584,34 @@
     </border>
     <border>
       <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -591,7 +626,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -746,9 +781,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -765,7 +809,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
@@ -813,7 +857,7 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000002-1185-4C1A-B1A4-BC1C676DBECF}"/>
               </c:ext>
@@ -829,7 +873,7 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-1185-4C1A-B1A4-BC1C676DBECF}"/>
               </c:ext>
@@ -845,7 +889,7 @@
               </c:spPr>
             </c:marker>
             <c:bubble3D val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000000-1185-4C1A-B1A4-BC1C676DBECF}"/>
               </c:ext>
@@ -863,7 +907,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>30</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>30.5</c:v>
@@ -875,7 +919,7 @@
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -905,7 +949,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-684E-462E-B6C5-08C4C156CB9E}"/>
             </c:ext>
@@ -919,11 +963,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="83477632"/>
-        <c:axId val="83479552"/>
+        <c:axId val="66735104"/>
+        <c:axId val="66753664"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="83477632"/>
+        <c:axId val="66735104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -954,12 +998,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83479552"/>
+        <c:crossAx val="66753664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="83479552"/>
+        <c:axId val="66753664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -990,7 +1034,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83477632"/>
+        <c:crossAx val="66735104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1013,7 +1057,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
   <c:roundedCorners val="0"/>
@@ -1070,7 +1114,7 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1100,7 +1144,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-3913-4CCA-937B-BFE2918FD451}"/>
             </c:ext>
@@ -1132,7 +1176,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>18</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>9</c:v>
@@ -1174,7 +1218,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-3913-4CCA-937B-BFE2918FD451}"/>
             </c:ext>
@@ -1248,7 +1292,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-3913-4CCA-937B-BFE2918FD451}"/>
             </c:ext>
@@ -1262,11 +1306,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="83514112"/>
-        <c:axId val="83515648"/>
+        <c:axId val="66777088"/>
+        <c:axId val="66779008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="83514112"/>
+        <c:axId val="66777088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1295,12 +1339,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83515648"/>
+        <c:crossAx val="66779008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="83515648"/>
+        <c:axId val="66779008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1330,7 +1374,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83514112"/>
+        <c:crossAx val="66777088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1418,9 +1462,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Larissa">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1458,9 +1502,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Larissa">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1495,7 +1539,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1530,7 +1574,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Larissa">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1710,7 +1754,7 @@
   <dimension ref="C1:M35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1759,14 +1803,14 @@
         <v>4</v>
       </c>
       <c r="F3" s="21">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="G3" s="22">
         <v>8</v>
       </c>
       <c r="H3" s="27">
         <f>E3+F3+G3</f>
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="I3" s="38">
         <v>98.77</v>
@@ -1875,11 +1919,11 @@
         <v>4</v>
       </c>
       <c r="G7" s="26">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H7" s="45">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="I7" s="41">
         <v>28.22</v>
@@ -1912,9 +1956,17 @@
       <c r="E9" s="21">
         <v>3</v>
       </c>
-      <c r="F9" s="21"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="46"/>
+      <c r="F9" s="21">
+        <f>2.5+4+0.5+0.5+2+3+5.5+3.5+8</f>
+        <v>29.5</v>
+      </c>
+      <c r="G9" s="22">
+        <v>1.5</v>
+      </c>
+      <c r="H9" s="61">
+        <f>E9+F9+G9</f>
+        <v>34</v>
+      </c>
       <c r="I9" s="47">
         <v>88.81</v>
       </c>
@@ -1933,9 +1985,16 @@
       <c r="E10" s="23">
         <v>2</v>
       </c>
-      <c r="F10" s="23"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="28"/>
+      <c r="F10" s="23">
+        <v>20</v>
+      </c>
+      <c r="G10" s="24">
+        <v>1</v>
+      </c>
+      <c r="H10" s="60">
+        <f t="shared" ref="H10:H12" si="1">E10+F10+G10</f>
+        <v>23</v>
+      </c>
       <c r="I10" s="42">
         <v>68.89</v>
       </c>
@@ -1954,9 +2013,17 @@
       <c r="E11" s="23">
         <v>2</v>
       </c>
-      <c r="F11" s="23"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="28"/>
+      <c r="F11" s="23">
+        <f>1.5+2+5+8</f>
+        <v>16.5</v>
+      </c>
+      <c r="G11" s="24">
+        <v>1.5</v>
+      </c>
+      <c r="H11" s="46">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
       <c r="I11" s="42">
         <v>42.33</v>
       </c>
@@ -1975,9 +2042,17 @@
       <c r="E12" s="29">
         <v>1.5</v>
       </c>
-      <c r="F12" s="29"/>
-      <c r="G12" s="30"/>
-      <c r="H12" s="31"/>
+      <c r="F12" s="29">
+        <f>1+4+0.5</f>
+        <v>5.5</v>
+      </c>
+      <c r="G12" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="H12" s="62">
+        <f t="shared" si="1"/>
+        <v>7.5</v>
+      </c>
       <c r="I12" s="43">
         <v>22.41</v>
       </c>

</xml_diff>

<commit_message>
Update FP for final
</commit_message>
<xml_diff>
--- a/usecases/Usecase doc.xlsx
+++ b/usecases/Usecase doc.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
   <si>
     <t>UC</t>
   </si>
@@ -103,6 +103,9 @@
   </si>
   <si>
     <t>Der erste Graph zeigt 3 Ausreißer auf. Der gelbe Ausreißer (View Instruction) war mit weniger Aufwand zu meistern. Dies liegt daran, dass die Oberfläche für die Spielanleitung meist generiert wurde.                                                                                                                                              Der grüne Ausreißer (View Wiki) war nach den Function Points zu aufwändig. Das lag daran, dass der Use Case mehr aus Dokumentation bestand (siehe 2ter Graph) als Entwicklung und weil die Dokumentation viel Aufwändiger war als zu begin vermutet. Es mussten zu jedem spielbaren Charakter (102 Figuren) viele Informationen, Beschreibungstexte und Bilder aus unterschiedlichen Quellen herangezogen werden, damit die Daten richtig sind!                                                                                                                                                       Der rote Ausreißer (Gamemode 1) war in ca. 30 Stunden fertiggestellt. Laut den Function Points sollten das mehr als 60 Stunden sein! Eine gute Begründung warum wir "nur" 30 Stunden benötigt haben, haben wir nicht!</t>
+  </si>
+  <si>
+    <t>In den einzelnen UC befindet sich die Beschreibung/Erklärung, warum die FP diesen Betrag haben.</t>
   </si>
 </sst>
 </file>
@@ -745,6 +748,15 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -780,15 +792,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -963,11 +966,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="66735104"/>
-        <c:axId val="66753664"/>
+        <c:axId val="83774464"/>
+        <c:axId val="83793024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="66735104"/>
+        <c:axId val="83774464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -998,12 +1001,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66753664"/>
+        <c:crossAx val="83793024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="66753664"/>
+        <c:axId val="83793024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1034,7 +1037,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66735104"/>
+        <c:crossAx val="83774464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1306,11 +1309,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="66777088"/>
-        <c:axId val="66779008"/>
+        <c:axId val="83816448"/>
+        <c:axId val="83818368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="66777088"/>
+        <c:axId val="83816448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1339,12 +1342,12 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66779008"/>
+        <c:crossAx val="83818368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="66779008"/>
+        <c:axId val="83818368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1374,7 +1377,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="66777088"/>
+        <c:crossAx val="83816448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1753,8 +1756,8 @@
   </sheetPr>
   <dimension ref="C1:M35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1934,16 +1937,16 @@
       <c r="K7" s="34"/>
     </row>
     <row r="8" spans="3:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="48" t="s">
+      <c r="C8" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="49"/>
-      <c r="I8" s="49"/>
-      <c r="J8" s="50"/>
+      <c r="D8" s="52"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="52"/>
+      <c r="H8" s="52"/>
+      <c r="I8" s="52"/>
+      <c r="J8" s="53"/>
       <c r="K8" s="35"/>
     </row>
     <row r="9" spans="3:13" x14ac:dyDescent="0.25">
@@ -1963,9 +1966,8 @@
       <c r="G9" s="22">
         <v>1.5</v>
       </c>
-      <c r="H9" s="61">
-        <f>E9+F9+G9</f>
-        <v>34</v>
+      <c r="H9" s="49">
+        <v>36</v>
       </c>
       <c r="I9" s="47">
         <v>88.81</v>
@@ -1991,9 +1993,8 @@
       <c r="G10" s="24">
         <v>1</v>
       </c>
-      <c r="H10" s="60">
-        <f t="shared" ref="H10:H12" si="1">E10+F10+G10</f>
-        <v>23</v>
+      <c r="H10" s="48">
+        <v>24</v>
       </c>
       <c r="I10" s="42">
         <v>68.89</v>
@@ -2021,7 +2022,7 @@
         <v>1.5</v>
       </c>
       <c r="H11" s="46">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="H10:H12" si="1">E11+F11+G11</f>
         <v>20</v>
       </c>
       <c r="I11" s="42">
@@ -2049,7 +2050,7 @@
       <c r="G12" s="30">
         <v>0.5</v>
       </c>
-      <c r="H12" s="62">
+      <c r="H12" s="50">
         <f t="shared" si="1"/>
         <v>7.5</v>
       </c>
@@ -2076,106 +2077,111 @@
       <c r="D14" s="20"/>
     </row>
     <row r="15" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C15" s="51" t="s">
+      <c r="C15" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="52"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="52"/>
-      <c r="G15" s="52"/>
-      <c r="H15" s="52"/>
-      <c r="I15" s="52"/>
-      <c r="J15" s="53"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="55"/>
+      <c r="H15" s="55"/>
+      <c r="I15" s="55"/>
+      <c r="J15" s="56"/>
     </row>
     <row r="16" spans="3:13" x14ac:dyDescent="0.25">
-      <c r="C16" s="54"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="55"/>
-      <c r="F16" s="55"/>
-      <c r="G16" s="55"/>
-      <c r="H16" s="55"/>
-      <c r="I16" s="55"/>
-      <c r="J16" s="56"/>
+      <c r="C16" s="57"/>
+      <c r="D16" s="58"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="58"/>
+      <c r="G16" s="58"/>
+      <c r="H16" s="58"/>
+      <c r="I16" s="58"/>
+      <c r="J16" s="59"/>
     </row>
     <row r="17" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C17" s="54"/>
-      <c r="D17" s="55"/>
-      <c r="E17" s="55"/>
-      <c r="F17" s="55"/>
-      <c r="G17" s="55"/>
-      <c r="H17" s="55"/>
-      <c r="I17" s="55"/>
-      <c r="J17" s="56"/>
+      <c r="C17" s="57"/>
+      <c r="D17" s="58"/>
+      <c r="E17" s="58"/>
+      <c r="F17" s="58"/>
+      <c r="G17" s="58"/>
+      <c r="H17" s="58"/>
+      <c r="I17" s="58"/>
+      <c r="J17" s="59"/>
     </row>
     <row r="18" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C18" s="54"/>
-      <c r="D18" s="55"/>
-      <c r="E18" s="55"/>
-      <c r="F18" s="55"/>
-      <c r="G18" s="55"/>
-      <c r="H18" s="55"/>
-      <c r="I18" s="55"/>
-      <c r="J18" s="56"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="58"/>
+      <c r="E18" s="58"/>
+      <c r="F18" s="58"/>
+      <c r="G18" s="58"/>
+      <c r="H18" s="58"/>
+      <c r="I18" s="58"/>
+      <c r="J18" s="59"/>
     </row>
     <row r="19" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C19" s="54"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="55"/>
-      <c r="F19" s="55"/>
-      <c r="G19" s="55"/>
-      <c r="H19" s="55"/>
-      <c r="I19" s="55"/>
-      <c r="J19" s="56"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="58"/>
+      <c r="E19" s="58"/>
+      <c r="F19" s="58"/>
+      <c r="G19" s="58"/>
+      <c r="H19" s="58"/>
+      <c r="I19" s="58"/>
+      <c r="J19" s="59"/>
     </row>
     <row r="20" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C20" s="54"/>
-      <c r="D20" s="55"/>
-      <c r="E20" s="55"/>
-      <c r="F20" s="55"/>
-      <c r="G20" s="55"/>
-      <c r="H20" s="55"/>
-      <c r="I20" s="55"/>
-      <c r="J20" s="56"/>
+      <c r="C20" s="57"/>
+      <c r="D20" s="58"/>
+      <c r="E20" s="58"/>
+      <c r="F20" s="58"/>
+      <c r="G20" s="58"/>
+      <c r="H20" s="58"/>
+      <c r="I20" s="58"/>
+      <c r="J20" s="59"/>
     </row>
     <row r="21" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C21" s="54"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="55"/>
-      <c r="F21" s="55"/>
-      <c r="G21" s="55"/>
-      <c r="H21" s="55"/>
-      <c r="I21" s="55"/>
-      <c r="J21" s="56"/>
+      <c r="C21" s="57"/>
+      <c r="D21" s="58"/>
+      <c r="E21" s="58"/>
+      <c r="F21" s="58"/>
+      <c r="G21" s="58"/>
+      <c r="H21" s="58"/>
+      <c r="I21" s="58"/>
+      <c r="J21" s="59"/>
     </row>
     <row r="22" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C22" s="54"/>
-      <c r="D22" s="55"/>
-      <c r="E22" s="55"/>
-      <c r="F22" s="55"/>
-      <c r="G22" s="55"/>
-      <c r="H22" s="55"/>
-      <c r="I22" s="55"/>
-      <c r="J22" s="56"/>
+      <c r="C22" s="57"/>
+      <c r="D22" s="58"/>
+      <c r="E22" s="58"/>
+      <c r="F22" s="58"/>
+      <c r="G22" s="58"/>
+      <c r="H22" s="58"/>
+      <c r="I22" s="58"/>
+      <c r="J22" s="59"/>
     </row>
     <row r="23" spans="3:10" x14ac:dyDescent="0.25">
-      <c r="C23" s="54"/>
-      <c r="D23" s="55"/>
-      <c r="E23" s="55"/>
-      <c r="F23" s="55"/>
-      <c r="G23" s="55"/>
-      <c r="H23" s="55"/>
-      <c r="I23" s="55"/>
-      <c r="J23" s="56"/>
+      <c r="C23" s="57"/>
+      <c r="D23" s="58"/>
+      <c r="E23" s="58"/>
+      <c r="F23" s="58"/>
+      <c r="G23" s="58"/>
+      <c r="H23" s="58"/>
+      <c r="I23" s="58"/>
+      <c r="J23" s="59"/>
     </row>
     <row r="24" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="57"/>
-      <c r="D24" s="58"/>
-      <c r="E24" s="58"/>
-      <c r="F24" s="58"/>
-      <c r="G24" s="58"/>
-      <c r="H24" s="58"/>
-      <c r="I24" s="58"/>
-      <c r="J24" s="59"/>
+      <c r="C24" s="60"/>
+      <c r="D24" s="61"/>
+      <c r="E24" s="61"/>
+      <c r="F24" s="61"/>
+      <c r="G24" s="61"/>
+      <c r="H24" s="61"/>
+      <c r="I24" s="61"/>
+      <c r="J24" s="62"/>
+    </row>
+    <row r="26" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="27" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C27" s="17" t="s">

</xml_diff>